<commit_message>
Common: Prepared another piece of data structure
</commit_message>
<xml_diff>
--- a/fixtures/mods.xlsx
+++ b/fixtures/mods.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C62D37C4-300F-42A6-BFFF-07221D4700E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8D665E1-7404-4D2B-BDC5-C8D16C6E9B28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2670" yWindow="5595" windowWidth="23955" windowHeight="13320" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16230" yWindow="2850" windowWidth="35085" windowHeight="18390" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tabs" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
   <si>
     <t>tab</t>
   </si>
@@ -37,9 +37,6 @@
     <t>mods</t>
   </si>
   <si>
-    <t>PuffSmith\Mod\Import\ModImport</t>
-  </si>
-  <si>
     <t>vendor</t>
   </si>
   <si>
@@ -77,6 +74,39 @@
   </si>
   <si>
     <t>power</t>
+  </si>
+  <si>
+    <t>mod</t>
+  </si>
+  <si>
+    <t>cost</t>
+  </si>
+  <si>
+    <t>voltage</t>
+  </si>
+  <si>
+    <t>cells</t>
+  </si>
+  <si>
+    <t>18650, 20700, 21700</t>
+  </si>
+  <si>
+    <t>18650, 18350</t>
+  </si>
+  <si>
+    <t>21700</t>
+  </si>
+  <si>
+    <t>Pulse II</t>
+  </si>
+  <si>
+    <t>Vandy Vape</t>
+  </si>
+  <si>
+    <t>Prestige MIXX</t>
+  </si>
+  <si>
+    <t>Aspire</t>
   </si>
 </sst>
 </file>
@@ -131,9 +161,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Nadpis 2" xfId="1" builtinId="17"/>
@@ -418,7 +453,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -440,7 +475,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -450,87 +485,184 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0888C51-D22A-4EB9-B572-2B7661763B22}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.140625" customWidth="1"/>
     <col min="2" max="2" width="27" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="23.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="C2" s="5">
+        <v>100</v>
+      </c>
+      <c r="D2" s="5">
+        <v>3.7</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="5">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" s="5">
+        <v>25</v>
+      </c>
+      <c r="D3" s="5">
+        <v>3.7</v>
+      </c>
+      <c r="E3" s="3">
+        <v>18350</v>
+      </c>
+      <c r="F3" s="5">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="C3">
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="5">
+        <v>70</v>
+      </c>
+      <c r="D4" s="5">
+        <v>3.7</v>
+      </c>
+      <c r="E4" s="3">
+        <v>18650</v>
+      </c>
+      <c r="F4" s="5">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="5">
+        <v>50</v>
+      </c>
+      <c r="D5" s="5">
+        <v>3.7</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="5">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="5">
+        <v>80</v>
+      </c>
+      <c r="D6" s="5">
+        <v>3.7</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="5">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="5">
+        <v>95</v>
+      </c>
+      <c r="D7" s="5">
+        <v>3.7</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="5">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6">
-        <v>80</v>
+      <c r="C8" s="5">
+        <v>60</v>
+      </c>
+      <c r="D8" s="5">
+        <v>3.7</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="5">
+        <v>125</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>